<commit_message>
Use SSEN instead of SSEPD.
</commit_message>
<xml_diff>
--- a/models/Market domain data.xlsx
+++ b/models/Market domain data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28000" windowHeight="12860" tabRatio="500"/>
@@ -499,12 +499,6 @@
     <t>Effective from</t>
   </si>
   <si>
-    <t>SSEPD SEPD</t>
-  </si>
-  <si>
-    <t>SSEPD SHEPD</t>
-  </si>
-  <si>
     <t>File name</t>
   </si>
   <si>
@@ -533,6 +527,12 @@
   </si>
   <si>
     <t>G2 Energy Networks (not yet active)</t>
+  </si>
+  <si>
+    <t>SSEN SEPD</t>
+  </si>
+  <si>
+    <t>SSEN SHEPD</t>
   </si>
 </sst>
 </file>
@@ -1389,7 +1389,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1410,13 +1410,13 @@
   <sheetData>
     <row r="1" spans="1:12" s="6" customFormat="1" ht="42">
       <c r="A1" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>132</v>
@@ -1425,19 +1425,19 @@
         <v>133</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>162</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>164</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>127</v>
@@ -1641,7 +1641,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>68</v>
@@ -1679,7 +1679,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>45</v>
@@ -2208,7 +2208,7 @@
         <v>138</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="1"/>
@@ -2230,7 +2230,7 @@
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="1"/>

</xml_diff>

<commit_message>
Market domain data update.
</commit_message>
<xml_diff>
--- a/models/Market domain data.xlsx
+++ b/models/Market domain data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28000" windowHeight="12860" tabRatio="500"/>
@@ -11,7 +11,7 @@
     <sheet name="Measurement Classes" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Distributors and GSP Groups'!$A$1:$L$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Distributors and GSP Groups'!$A$1:$L$26</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="173">
   <si>
     <t>WPD EastM</t>
   </si>
@@ -533,6 +533,15 @@
   </si>
   <si>
     <t>SSEN SHEPD</t>
+  </si>
+  <si>
+    <t>Dragon</t>
+  </si>
+  <si>
+    <t>Utility Distribution Networks (not yet active)</t>
+  </si>
+  <si>
+    <t>Utility Distribution Networks Limited</t>
   </si>
 </sst>
 </file>
@@ -605,8 +614,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="193">
+  <cellStyleXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -832,7 +845,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="193">
+  <cellStyles count="197">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -929,6 +942,8 @@
     <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1025,6 +1040,8 @@
     <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
@@ -1383,13 +1400,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2094,26 +2111,28 @@
       <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="C20" s="1" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="1"/>
       <c r="F20" s="2"/>
       <c r="G20" s="1"/>
       <c r="H20" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L20" s="11">
-        <v>6489447</v>
+        <v>7330883</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -2121,27 +2140,27 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="1"/>
       <c r="F21" s="2"/>
       <c r="G21" s="1"/>
       <c r="H21" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="L21" s="11">
-        <v>7330883</v>
+        <v>6684589</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -2149,27 +2168,27 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="1"/>
       <c r="F22" s="2"/>
       <c r="G22" s="1"/>
       <c r="H22" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="L22" s="11">
-        <v>6684589</v>
+        <v>6339585</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -2177,27 +2196,23 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>135</v>
+        <v>167</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="1"/>
       <c r="F23" s="2"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="2">
-        <v>31</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>137</v>
-      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="L23" s="11">
-        <v>6339585</v>
+        <v>9633506</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -2205,10 +2220,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="1"/>
@@ -2218,15 +2233,15 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
       <c r="L24" s="11">
-        <v>9633506</v>
+        <v>10068882</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="2">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
@@ -2247,12 +2262,38 @@
       </c>
     </row>
     <row r="26" spans="1:12">
-      <c r="L26" s="3"/>
+      <c r="A26" s="2">
+        <v>99</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="2">
+        <v>28</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L26" s="11">
+        <v>6489447</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="L27" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L25">
-    <sortState ref="A2:L25">
-      <sortCondition ref="A1:A25"/>
+  <autoFilter ref="A1:L26">
+    <sortState ref="A2:L26">
+      <sortCondition ref="A1:A26"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>